<commit_message>
Popravio format datuma u dnevniku sastajanja
</commit_message>
<xml_diff>
--- a/dnevnikSastajanja.xlsx
+++ b/dnevnikSastajanja.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vlado\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matep\git\pets-only-zg\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>Sodić</t>
   </si>
@@ -94,12 +94,15 @@
   </si>
   <si>
     <t>Osnovne funkcionalnosti aplikacije i use caseovi</t>
+  </si>
+  <si>
+    <t>22.10.2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -229,6 +232,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -241,30 +268,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -283,15 +286,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -307,7 +310,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -602,413 +605,410 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="21"/>
-    </row>
-    <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="15" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="16"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="5" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="14"/>
       <c r="G3" s="17"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="5" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="14"/>
       <c r="G4" s="17"/>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="14"/>
       <c r="G5" s="17"/>
       <c r="H5" s="18"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="17"/>
       <c r="H6" s="18"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="19"/>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="15" t="s">
         <v>21</v>
       </c>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="5" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="17"/>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="5" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="14"/>
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="5" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="5" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="17"/>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="19"/>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="22">
-        <v>43030</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="15" t="s">
         <v>20</v>
       </c>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="5" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="17"/>
       <c r="H15" s="18"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14"/>
       <c r="G16" s="17"/>
       <c r="H16" s="18"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="6"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="17"/>
       <c r="H17" s="18"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="14"/>
       <c r="G18" s="17"/>
       <c r="H18" s="18"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="19"/>
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="12" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="3" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="4"/>
+      <c r="F20" s="12"/>
       <c r="G20" s="15" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="5" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="6"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="17"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="5" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="6"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="17"/>
       <c r="H22" s="18"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="6"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="17"/>
       <c r="H23" s="18"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="6"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="14"/>
       <c r="G24" s="17"/>
       <c r="H24" s="18"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="19"/>
       <c r="H25" s="20"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="12"/>
       <c r="G26" s="15"/>
       <c r="H26" s="16"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="6"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="14"/>
       <c r="G27" s="17"/>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="6"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="14"/>
       <c r="G28" s="17"/>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="6"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="14"/>
       <c r="G29" s="17"/>
       <c r="H29" s="18"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="6"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="14"/>
       <c r="G30" s="17"/>
       <c r="H30" s="18"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="4"/>
       <c r="G31" s="19"/>
       <c r="H31" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A26:B31"/>
-    <mergeCell ref="C26:D31"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A20:B25"/>
-    <mergeCell ref="C20:D25"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G2:H7"/>
+    <mergeCell ref="G8:H13"/>
+    <mergeCell ref="G14:H19"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D7"/>
+    <mergeCell ref="A2:B7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="G20:H25"/>
     <mergeCell ref="G26:H31"/>
     <mergeCell ref="A8:B13"/>
@@ -1023,25 +1023,28 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C2:D7"/>
-    <mergeCell ref="A2:B7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G2:H7"/>
-    <mergeCell ref="G8:H13"/>
-    <mergeCell ref="G14:H19"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A20:B25"/>
+    <mergeCell ref="C20:D25"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A26:B31"/>
+    <mergeCell ref="C26:D31"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F31" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Sudionici</formula1>
     </dataValidation>
   </dataValidations>
@@ -1050,49 +1053,49 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B3:B8"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>